<commit_message>
feat: update DR compute/licensing, backup capacity fixes, new PDFs + migrations
</commit_message>
<xml_diff>
--- a/public/assets/ECSandBackup_Template_AutoCalculation_v1.250804.xlsx
+++ b/public/assets/ECSandBackup_Template_AutoCalculation_v1.250804.xlsx
@@ -610,7 +610,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -890,8 +890,8 @@
   </sheetPr>
   <dimension ref="A1:AU1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA5" activeCellId="0" sqref="AA5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AQ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AW4" activeCellId="0" sqref="AW4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1240,7 +1240,7 @@
       <c r="Y4" s="14"/>
       <c r="Z4" s="14"/>
       <c r="AA4" s="18" t="n">
-        <f aca="false">(W4+X4+Y4+Z4)*T4</f>
+        <f aca="false">(W4+X4+Y4+Z4)</f>
         <v>0</v>
       </c>
       <c r="AB4" s="18" t="n">
@@ -1331,7 +1331,7 @@
       <c r="Y5" s="14"/>
       <c r="Z5" s="14"/>
       <c r="AA5" s="18" t="n">
-        <f aca="false">(W5+X5+Y5+Z5)*T5</f>
+        <f aca="false">(W5+X5+Y5+Z5)</f>
         <v>0</v>
       </c>
       <c r="AB5" s="18" t="n">
@@ -1422,7 +1422,7 @@
       <c r="Y6" s="14"/>
       <c r="Z6" s="14"/>
       <c r="AA6" s="18" t="n">
-        <f aca="false">(W6+X6+Y6+Z6)*T6</f>
+        <f aca="false">(W6+X6+Y6+Z6)</f>
         <v>0</v>
       </c>
       <c r="AB6" s="18" t="n">
@@ -1513,7 +1513,7 @@
       <c r="Y7" s="14"/>
       <c r="Z7" s="14"/>
       <c r="AA7" s="18" t="n">
-        <f aca="false">(W7+X7+Y7+Z7)*T7</f>
+        <f aca="false">(W7+X7+Y7+Z7)</f>
         <v>0</v>
       </c>
       <c r="AB7" s="18" t="n">
@@ -1606,7 +1606,7 @@
       <c r="Y8" s="14"/>
       <c r="Z8" s="14"/>
       <c r="AA8" s="18" t="n">
-        <f aca="false">(W8+X8+Y8+Z8)*T8</f>
+        <f aca="false">(W8+X8+Y8+Z8)</f>
         <v>0</v>
       </c>
       <c r="AB8" s="18" t="n">
@@ -1699,7 +1699,7 @@
       <c r="Y9" s="14"/>
       <c r="Z9" s="14"/>
       <c r="AA9" s="18" t="n">
-        <f aca="false">(W9+X9+Y9+Z9)*T9</f>
+        <f aca="false">(W9+X9+Y9+Z9)</f>
         <v>0</v>
       </c>
       <c r="AB9" s="18" t="n">
@@ -1792,7 +1792,7 @@
       <c r="Y10" s="14"/>
       <c r="Z10" s="14"/>
       <c r="AA10" s="18" t="n">
-        <f aca="false">(W10+X10+Y10+Z10)*T10</f>
+        <f aca="false">(W10+X10+Y10+Z10)</f>
         <v>0</v>
       </c>
       <c r="AB10" s="18" t="n">
@@ -1885,7 +1885,7 @@
       <c r="Y11" s="14"/>
       <c r="Z11" s="14"/>
       <c r="AA11" s="18" t="n">
-        <f aca="false">(W11+X11+Y11+Z11)*T11</f>
+        <f aca="false">(W11+X11+Y11+Z11)</f>
         <v>0</v>
       </c>
       <c r="AB11" s="18" t="n">
@@ -1978,7 +1978,7 @@
       <c r="Y12" s="14"/>
       <c r="Z12" s="14"/>
       <c r="AA12" s="18" t="n">
-        <f aca="false">(W12+X12+Y12+Z12)*T12</f>
+        <f aca="false">(W12+X12+Y12+Z12)</f>
         <v>0</v>
       </c>
       <c r="AB12" s="18" t="n">
@@ -2071,7 +2071,7 @@
       <c r="Y13" s="14"/>
       <c r="Z13" s="14"/>
       <c r="AA13" s="18" t="n">
-        <f aca="false">(W13+X13+Y13+Z13)*T13</f>
+        <f aca="false">(W13+X13+Y13+Z13)</f>
         <v>0</v>
       </c>
       <c r="AB13" s="18" t="n">
@@ -2164,7 +2164,7 @@
       <c r="Y14" s="14"/>
       <c r="Z14" s="14"/>
       <c r="AA14" s="18" t="n">
-        <f aca="false">(W14+X14+Y14+Z14)*T14</f>
+        <f aca="false">(W14+X14+Y14+Z14)</f>
         <v>0</v>
       </c>
       <c r="AB14" s="18" t="n">
@@ -2257,7 +2257,7 @@
       <c r="Y15" s="14"/>
       <c r="Z15" s="14"/>
       <c r="AA15" s="18" t="n">
-        <f aca="false">(W15+X15+Y15+Z15)*T15</f>
+        <f aca="false">(W15+X15+Y15+Z15)</f>
         <v>0</v>
       </c>
       <c r="AB15" s="18" t="n">
@@ -2350,7 +2350,7 @@
       <c r="Y16" s="14"/>
       <c r="Z16" s="14"/>
       <c r="AA16" s="18" t="n">
-        <f aca="false">(W16+X16+Y16+Z16)*T16</f>
+        <f aca="false">(W16+X16+Y16+Z16)</f>
         <v>0</v>
       </c>
       <c r="AB16" s="18" t="n">
@@ -2443,7 +2443,7 @@
       <c r="Y17" s="14"/>
       <c r="Z17" s="14"/>
       <c r="AA17" s="18" t="n">
-        <f aca="false">(W17+X17+Y17+Z17)*T17</f>
+        <f aca="false">(W17+X17+Y17+Z17)</f>
         <v>0</v>
       </c>
       <c r="AB17" s="18" t="n">
@@ -2536,7 +2536,7 @@
       <c r="Y18" s="14"/>
       <c r="Z18" s="14"/>
       <c r="AA18" s="18" t="n">
-        <f aca="false">(W18+X18+Y18+Z18)*T18</f>
+        <f aca="false">(W18+X18+Y18+Z18)</f>
         <v>0</v>
       </c>
       <c r="AB18" s="18" t="n">
@@ -2629,7 +2629,7 @@
       <c r="Y19" s="14"/>
       <c r="Z19" s="14"/>
       <c r="AA19" s="18" t="n">
-        <f aca="false">(W19+X19+Y19+Z19)*T19</f>
+        <f aca="false">(W19+X19+Y19+Z19)</f>
         <v>0</v>
       </c>
       <c r="AB19" s="18" t="n">
@@ -2722,7 +2722,7 @@
       <c r="Y20" s="14"/>
       <c r="Z20" s="14"/>
       <c r="AA20" s="18" t="n">
-        <f aca="false">(W20+X20+Y20+Z20)*T20</f>
+        <f aca="false">(W20+X20+Y20+Z20)</f>
         <v>0</v>
       </c>
       <c r="AB20" s="18" t="n">
@@ -2815,7 +2815,7 @@
       <c r="Y21" s="14"/>
       <c r="Z21" s="14"/>
       <c r="AA21" s="18" t="n">
-        <f aca="false">(W21+X21+Y21+Z21)*T21</f>
+        <f aca="false">(W21+X21+Y21+Z21)</f>
         <v>0</v>
       </c>
       <c r="AB21" s="18" t="n">
@@ -2908,7 +2908,7 @@
       <c r="Y22" s="14"/>
       <c r="Z22" s="14"/>
       <c r="AA22" s="18" t="n">
-        <f aca="false">(W22+X22+Y22+Z22)*T22</f>
+        <f aca="false">(W22+X22+Y22+Z22)</f>
         <v>0</v>
       </c>
       <c r="AB22" s="18" t="n">
@@ -3001,7 +3001,7 @@
       <c r="Y23" s="14"/>
       <c r="Z23" s="14"/>
       <c r="AA23" s="18" t="n">
-        <f aca="false">(W23+X23+Y23+Z23)*T23</f>
+        <f aca="false">(W23+X23+Y23+Z23)</f>
         <v>0</v>
       </c>
       <c r="AB23" s="18" t="n">
@@ -3094,7 +3094,7 @@
       <c r="Y24" s="14"/>
       <c r="Z24" s="14"/>
       <c r="AA24" s="18" t="n">
-        <f aca="false">(W24+X24+Y24+Z24)*T24</f>
+        <f aca="false">(W24+X24+Y24+Z24)</f>
         <v>0</v>
       </c>
       <c r="AB24" s="18" t="n">
@@ -3187,7 +3187,7 @@
       <c r="Y25" s="14"/>
       <c r="Z25" s="14"/>
       <c r="AA25" s="18" t="n">
-        <f aca="false">(W25+X25+Y25+Z25)*T25</f>
+        <f aca="false">(W25+X25+Y25+Z25)</f>
         <v>0</v>
       </c>
       <c r="AB25" s="18" t="n">
@@ -3280,7 +3280,7 @@
       <c r="Y26" s="14"/>
       <c r="Z26" s="14"/>
       <c r="AA26" s="18" t="n">
-        <f aca="false">(W26+X26+Y26+Z26)*T26</f>
+        <f aca="false">(W26+X26+Y26+Z26)</f>
         <v>0</v>
       </c>
       <c r="AB26" s="18" t="n">
@@ -3373,7 +3373,7 @@
       <c r="Y27" s="14"/>
       <c r="Z27" s="14"/>
       <c r="AA27" s="18" t="n">
-        <f aca="false">(W27+X27+Y27+Z27)*T27</f>
+        <f aca="false">(W27+X27+Y27+Z27)</f>
         <v>0</v>
       </c>
       <c r="AB27" s="18" t="n">
@@ -3466,7 +3466,7 @@
       <c r="Y28" s="14"/>
       <c r="Z28" s="14"/>
       <c r="AA28" s="18" t="n">
-        <f aca="false">(W28+X28+Y28+Z28)*T28</f>
+        <f aca="false">(W28+X28+Y28+Z28)</f>
         <v>0</v>
       </c>
       <c r="AB28" s="18" t="n">
@@ -3559,7 +3559,7 @@
       <c r="Y29" s="14"/>
       <c r="Z29" s="14"/>
       <c r="AA29" s="18" t="n">
-        <f aca="false">(W29+X29+Y29+Z29)*T29</f>
+        <f aca="false">(W29+X29+Y29+Z29)</f>
         <v>0</v>
       </c>
       <c r="AB29" s="18" t="n">
@@ -3652,7 +3652,7 @@
       <c r="Y30" s="14"/>
       <c r="Z30" s="14"/>
       <c r="AA30" s="18" t="n">
-        <f aca="false">(W30+X30+Y30+Z30)*T30</f>
+        <f aca="false">(W30+X30+Y30+Z30)</f>
         <v>0</v>
       </c>
       <c r="AB30" s="18" t="n">
@@ -3745,7 +3745,7 @@
       <c r="Y31" s="14"/>
       <c r="Z31" s="14"/>
       <c r="AA31" s="18" t="n">
-        <f aca="false">(W31+X31+Y31+Z31)*T31</f>
+        <f aca="false">(W31+X31+Y31+Z31)</f>
         <v>0</v>
       </c>
       <c r="AB31" s="18" t="n">
@@ -3838,7 +3838,7 @@
       <c r="Y32" s="14"/>
       <c r="Z32" s="14"/>
       <c r="AA32" s="18" t="n">
-        <f aca="false">(W32+X32+Y32+Z32)*T32</f>
+        <f aca="false">(W32+X32+Y32+Z32)</f>
         <v>0</v>
       </c>
       <c r="AB32" s="18" t="n">

</xml_diff>